<commit_message>
feat: add good encounters
</commit_message>
<xml_diff>
--- a/data/randoms.xlsx
+++ b/data/randoms.xlsx
@@ -15,6 +15,7 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Bad Random Encounters (27)'!$A$1:$C$1000</definedName>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'Good Random Encounters (18)'!$A$1:$C$1000</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -1079,6 +1080,188 @@
         <sz val="7.0"/>
       </rPr>
       <t xml:space="preserve">Scenario:
+After a long day of intense battles in Cobot's Steam Arena (sponsored by BITS Artificial Services), you return to the comfort of the pilot dormitories. As you enter the communal lounge, you notice a group of fellow pilots engaged in a friendly sparring match.
+Eager to join in, you step into the makeshift ring and spar with your fellow pilots. The adrenaline rushes through your circuits as you exchange blows, honing your combat skills and reflexes. The camaraderie and competitive spirit create an uplifting atmosphere, energizing you.
+As the sparring session comes to an end, you find yourself invigorated and revitalized. The friendly exchanges have not only strengthened your bond with your fellow pilots but also boosted your confidence and endurance. Your body feels recharged, and your spirit soars high.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>BITS:
+Oh, I see. This is your way of socializing. Have you ever tried, umm, what was it called? Oh yes, talking? 
+Outcome:
+-Regenerated an EP</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx participates in a spirited sparring session with fellow pilots in the dormitories. The friendly combat invigorates him, resulting in an EP regeneration.
+Outcome:
+-Regenerated an EP</t>
+  </si>
+  <si>
+    <t>-Earned X Credits x4
+-Gained X HP x3
+-Gained X HP, Earned X Credits x1
+-Gained X HP, Earned X Credits, Regenerated an EP x1
+-Gained X HP, Regenerated an EP x1
+-Regenerated an EP x2
+-Regenerated two EPs x1
+-Regenerated all EPs x1
+-Upgraded your X to Gravitational Absorber (armor) x1
+-Upgraded your X to Super Duper Planet Blower (weapon) x1
+-Acquired X (armor) x1
+-Acquired X (weapon) x1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>Scenario:
+Amidst the hustle and bustle of the Hospital Wing in Cobot's Steam Arena (sponsored by BITS Artificial Services), you come across an intriguing medical research display. A renowned scientist, Dr. Aurora, stands by the exhibit, her eyes gleaming with curiosity and passion.
+Dr. Aurora invites you to explore her groundbreaking research on advanced bio-neural technology. As you delve deeper into the intricacies of her work, you uncover an innovative device known as the "Neural Resonance Enhancer."
+This extraordinary invention has the ability to enhance your neural connections, granting you greater mental acuity and reflexes. Dr. Aurora eagerly offers you the chance to experience the "Neural Resonance Enhancer" firsthand.
+With a sense of excitement, you agree to participate in her experiment. Dr. Aurora carefully connects the device to your Cobot's neural interface, and you feel a subtle surge of energy coursing through your circuits.
+The "Neural Resonance Enhancer" initiates a synchronized resonance with your consciousness, awakening dormant potential within. You sense a newfound clarity and focus, as if the entire arena's secrets lay bare before you.
+As you leave Dr. Aurora's display, you find your thoughts sharper and your responses quicker. The "Neural Resonance Enhancer" has left a lasting impact on your Cobot's neural pathways, granting you an advantage in Spintop's Cobot Rumble.</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">
+BITS:
+I did not know that you were so eager to join the experiments as a subject without knowing the outcome. I am creating a new dimension where organic life is impossible to sustain. Would you like to give it a spin?
+Outcome:
+-Regenerated an EP</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx ventures into the Hospital Wing, where he encounters Dr. Aurora and her revolutionary "Neural Resonance Enhancer." Eager to explore its potential, @xxx undergoes the experiment and emerges with heightened mental acuity.
+Outcome:
+-Regenerated an EP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>Scenario:
+With a determined look in your eyes, you step onto the sprawling training grounds of Cobot's Steam Arena (sponsored by BITS Artificial Services). The training ground is a hub of activity, with pilots and their Cobots honing their skills, pushing their limits, and preparing for upcoming battles.
+As you join the training session, you find yourself partnered with an experienced pilot known for their exceptional combat prowess. The seasoned pilot is impressed by your dedication and agrees to spar with you, offering valuable guidance throughout the practice session.
+In the intense battle that follows, you give your all, using every trick and technique you've learned over the years. The experienced pilot challenges you to adapt, improvise, and think strategically, pushing you to the limit. Through the spirited contest, you gain valuable combat experience, and your reflexes sharpen considerably.
+Recognizing your progress and determination, the seasoned pilot commends your efforts and shares a few of their most effective strategies. Their guidance proves invaluable, providing you with new approaches to confront your adversaries in the arena.
+As the training session comes to an end, you feel a surge of newfound confidence and pride in your abilities. The experience has not only honed your combat skills but also renewed your spirit for the battles ahead. Grateful for the valuable training and mentorship, you express your thanks to the experienced pilot.</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">
+BITS:
+Well, I am impressed. You look powerful, determined, and intimidating. You may actually prove deadly to your opponents after all. I'm impressed, indeed. 
+Outcome:
+-Regenerated two EPs</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx engages in a spirited training session on the training grounds of Cobot's Steam Arena. The mentorship of an experienced pilot not only sharpens his combat skills but also regenerates two EPs.
+Outcome:
+-Regenerated two EPs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">Scenario:
+Your Cobot has taken a beating after a battle in the arena, and you've sustained some minor injuries. Wasting no time, you head to the hospital wing of Cobot's Steam Arena (sponsored by BITS Artificial Services) for much-needed medical attention.
+As you enter the well-equipped hospital wing, the attentive medical staff quickly attends to your Cobot and assesses your injuries. The advanced medical technology in this facility is a marvel to behold, and you feel reassured by the skilled hands of the medical team.
+After a thorough examination, the doctors administer advanced treatments to repair your Cobot's damaged systems and initiate a series of specialized nanobot injections to accelerate your healing process. Within moments, you feel a surge of vitality coursing through your circuits as your injuries begin to mend.
+With a mix of relief and gratitude, you watch as your Cobot's health indicators start to stabilize and improve. The hospital wing's state-of-the-art facilities and the expertise of the medical team have undoubtedly expedited your recovery and restored your Cobot to its peak condition.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i val="0"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>BITS:
+Did you know that I've personally created the blueprints of each device and bot on the hospital wing? Aren't they just perfect? You're welcome.
+Outcome:
+-Gained 20 HP</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx receives expert medical attention in the hospital wing of Cobot's Steam Arena. Thanks to the advanced treatments, his Cobot's health is swiftly restored, and he is ready for the next battle.
+Outcome:
+-Gained X HP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">Scenario:
+After a rigorous training session at the Cobot's Steam Arena (sponsored by BITS Artificial Services), your stomach growls with hunger. You head to the bustling food court, a culinary paradise offering a wide array of delicious treats to satiate your appetite.
+As you browse through the various food stalls, the aromas of tantalizing dishes envelop your senses. It's a tough decision to make with so many mouthwatering options, but eventually, you settle on a hearty and nutritious meal that promises to rejuvenate your energy.
+With your plate in hand, you find a cozy corner to enjoy your well-deserved feast. Each bite fills you with satisfaction, and you feel your body being revitalized as the nourishing flavors work their magic. The meal not only pleases your taste buds but also serves as a perfect recovery after your intense training session.
+As you savor the last morsel, you feel a renewed sense of vigor and strength coursing through your circuits. The food court's culinary delights have not only satisfied your hunger but also reinvigorated your body, leaving you ready to face any challenges that lie ahead.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>BITS:
+Oh, Leia's Spoonful Happiness is a great place to eat. Sometimes I wish I could eat food. But again, being perfect is not easy, and being unable to eat food is a small price for being perfect.
+Outcome:
+-Gained 10 HP</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx indulges in a delightful meal at the food court, reaping the rewards of a nourishing feast. HP levels surge as the pilot's body rejuvenates.
+Outcome:
+-Gained X HP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">Scenario:
 As you navigate through the bustling streets of Cobot's Steam Arena (sponsored by BITS Artificial Services), a vibrant poster catches your attention. It announces the "Cobot Cosplay Contest" at Aether Avenue, a renowned landmark known for its lively atmosphere and entertainment.
 Intrigued by the idea of showcasing your creativity, you decide to enter the contest. Excitement courses through your circuits as you plan the perfect Cobot-inspired costume. You spend hours crafting the outfit, meticulously adding every detail to make it truly stand out.
 The day of the contest arrives, and you make your way to Aether Avenue, where the stage is set, and the audience is abuzz with anticipation. The atmosphere is electric as the judges examine each contestant with keen eyes. As the time for the results draws near, your heart pounds with nervous excitement.
@@ -1095,7 +1278,7 @@
       <t>BITS:
 I thought you were dressed as yourself; big, clunky, ugly, and oily. Apparently, I need to revisit the sense of beauty of my artificial dimension. If they chose you, there must be a problem with the codes.
 Outcome:
--Earned X Credits</t>
+-Earned 50 Credits</t>
     </r>
   </si>
   <si>
@@ -1103,52 +1286,6 @@
 @xxx shines on the stage of the Cobot Cosplay Contest at Aether Avenue with his costume. The judges are impressed by his creativity and award his with a generous sum of Credits.
 Outcome:
 -Earned X Credits</t>
-  </si>
-  <si>
-    <t>-Earned X Credits x4
--Gained X HP x3
--Gained X HP, Earned X Credits x1
--Gained X HP, Earned X Credits, Regenerated an EP x1
--Gained X HP, Regenerated an EP x1
--Regenerated an EP x2
--Regenerated two EPs x1
--Regerenated all EPs x1
--Upgraded your X to Gravitational Absorber (armor) x1
--Upgraded your X to Super Duper Planet Blower (weapon) x1
--Acquired X (armor) x1
--Acquired X (weapon) x1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">Scenario:
-After a long day of intense battles in Cobot's Steam Arena (sponsored by BITS Artificial Services), you return to the comfort of the pilot dormitories. As you enter the communal lounge, you notice a group of fellow pilots engaged in a friendly sparring match.
-Eager to join in, you step into the makeshift ring and spar with your fellow pilots. The adrenaline rushes through your circuits as you exchange blows, honing your combat skills and reflexes. The camaraderie and competitive spirit create an uplifting atmosphere, energizing you.
-As the sparring session comes to an end, you find yourself invigorated and revitalized. The friendly exchanges have not only strengthened your bond with your fellow pilots but also boosted your confidence and endurance. Your body feels recharged, and your spirit soars high.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>BITS:
-Oh, I see. This is your way of socializing. Have you ever tried, umm, what was it called? Oh yes, talking? 
-Outcome:
--Regenerated an EP</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx participates in a spirited sparring session with fellow pilots in the dormitories. The friendly combat invigorates him, resulting in an EP regeneration.
-Outcome:
--Regenerated an EP</t>
   </si>
   <si>
     <r>
@@ -1173,7 +1310,7 @@
       <t>BITS:
 Oh, I remember that Cobot! Its name was Boomer because it blew up every single Cobot it faced with its gigantic Super Duper Planet Blower. Ah, it was so good.
 Outcome:
--Gained X HP</t>
+-Gained 40 HP</t>
     </r>
   </si>
   <si>
@@ -1181,6 +1318,76 @@
 @xxx finds inspiration in an ancient figurine of a legendary Cobot warrior acquired from the souvenir shop. The connection to the past rejuvenates his spirit, resulting in a notable gain of HP.
 Outcome:
 -Gained X HP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>Scenario:
+Amidst the aroma of delectable delicacies and the chatter of fellow pilots in Cobot's Steam Arena (sponsored by BITS Artificial Services), you find yourself at the bustling Food Court, contemplating your dining options.
+As you peruse the various food stalls, your attention is drawn to an unassuming vending machine tucked in the corner. Unlike the others, this vending machine seems to radiate an aura of intelligence, with blinking lights and holographic equations swirling around it.
+Intrigued, you approach the machine, and it greets you with a cheerful holographic display. "Welcome, esteemed pilot! I am the Gourmettron 9000, an AI-powered vending machine with a passion for gastronomy and brain teasers."
+The Gourmettron 9000 offers you a unique proposition - a culinary challenge! It boasts a collection of exotic dishes from across the universe, each connected to a riddle or puzzle. If you successfully solve the riddle, the Gourmettron 9000 will treat you to an extraordinary meal and reward you with a generous amount of Credits.
+Eager for the opportunity, you accept the challenge and prepare to put your wits to the test. The Gourmettron 9000 presents you with an intricate puzzle, and you delve into the enigma, savoring the mental stimulation.
+With each step towards the solution, you can almost taste the victory. Moments later, your problem-solving prowess triumphs, and the Gourmettron 9000 commends you with a holographic applause.
+True to its word, the vending machine dispenses a delectable feast, and you indulge in the gastronomic delight. As you savor the culinary masterpiece, the Gourmettron 9000 credits your account with a generous sum, acknowledging your brilliance and culinary appreciation.</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">
+BITS:
+There are 47,989 different robots, bots, and drones in this artificial dimension that I've created. I programmed nearly half of them specifically to be puzzling and teasing. Out of 23,259 mechanic automaton riddle givers, you've found the most merciful one. Congratulations.
+Outcome:
+-Earned 75 Credits</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx faces an intellectual challenge at the Food Court as he encounters the Gourmettron 9000, an AI-powered vending machine. By skillfully solving the riddle, @xxx earns a generous reward of Credits and indulges in an exquisite feast.
+Outcome:
+-Earned X Credits</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">Scenario:
+In the farthest reaches of the Cobot's Steam Arena (sponsored by BITS Artificial Services), hidden behind layers of advanced holographic barriers, lies the enigmatic "Nebula Nexus." This elusive nexus is rumored to be an ancient source of boundless energy, capable of revitalizing even the most drained Cobots.
+As you embark on a daring expedition to locate the Nebula Nexus, whispers of its existence become more fervent. Many pilots have sought its rejuvenating powers, but few have ever returned to tell the tale. Undeterred, you follow a cryptic trail of clues left by those who came before, your determination fueling your journey.
+After navigating through treacherous terrain and solving intricate puzzles, you finally stand before the mesmerizing Nebula Nexus. A pulsating, iridescent cloud of energy envelops you and your Cobot, infusing you both with renewed vitality.
+In the embrace of the Nebula Nexus, time seems to slow, and you can feel every fiber of your Cobot's being reinvigorating. Your EPs, once depleted, now surge back to full capacity, as if the nexus itself grants you the power to push beyond your limits.
+With your Cobot revitalized and your spirits lifted, you step away from the Nebula Nexus, awestruck by the profound experience. You can't help but feel a sense of connection to this ancient source of energy, as if it recognizes and rewards the worthy pilots who seek its blessings.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>BITS:
+Nebula Nexus, have you been there? If so, how are you still alive? Even I don't prefer to explore that mysterious place. Yes, this dimension is my creation, but Nebula Nexus is a total mystery, even to me.
+Outcome:
+-Regenerated all EPs</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx embarks on a perilous quest to discover the legendary Nebula Nexus. A place of mystical energy said to restore the weary. The rewards of courage and determination are truly grand!
+Outcome:
+-Regenerated all EPs</t>
   </si>
   <si>
     <r>
@@ -1207,7 +1414,7 @@
       <t>BITS:
 That is actually a well-thought engine. I am going to take it from the mechanics' hand and patent it on behalf of BITS Artificial Services. In the end, this is my domain, you know.
 Outcome:
--Earned X Credits</t>
+-Earned 100 Credits</t>
     </r>
   </si>
   <si>
@@ -1215,106 +1422,6 @@
 @xxx witnesses a groundbreaking engine modification in the Cobot hangars and offers valuable feedback to the mechanics. His expertise is recognized, leading to a generous reward of Credits.
 Outcome:
 -Earned X Credits</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">Scenario:
-Your Cobot has taken a beating after a battle in the arena, and you've sustained some minor injuries. Wasting no time, you head to the hospital wing of Cobot's Steam Arena (sponsored by BITS Artificial Services) for much-needed medical attention.
-As you enter the well-equipped hospital wing, the attentive medical staff quickly attends to your Cobot and assesses your injuries. The advanced medical technology in this facility is a marvel to behold, and you feel reassured by the skilled hands of the medical team.
-After a thorough examination, the doctors administer advanced treatments to repair your Cobot's damaged systems and initiate a series of specialized nanobot injections to accelerate your healing process. Within moments, you feel a surge of vitality coursing through your circuits as your injuries begin to mend.
-With a mix of relief and gratitude, you watch as your Cobot's health indicators start to stabilize and improve. The hospital wing's state-of-the-art facilities and the expertise of the medical team have undoubtedly expedited your recovery and restored your Cobot to its peak condition.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i val="0"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>BITS:
-Did you know that I've personally created the blueprints of each device and bot on the hospital wing? Aren't they just perfect? You're welcome.
-Outcome:
--Gained X HP</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx receives expert medical attention in the hospital wing of Cobot's Steam Arena. Thanks to the advanced treatments, his Cobot's health is swiftly restored, and he is ready for the next battle.
-Outcome:
--Gained X HP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>Scenario:
-As you venture into the vast and bustling factories within Cobot's Steam Arena (sponsored by BITS Artificial Services), you find yourself amidst an impressive display of cutting-edge machinery and skilled technicians working tirelessly to produce the latest innovations in Cobot technology.
-Intrigued by the mesmerizing assembly lines and state-of-the-art production processes, you strike up a conversation with one of the friendly engineers. Impressed by your passion for Cobots and the arena, the engineer decides to show you around and offer some insider tips.
-As you explore the inner workings of the factory, you gain valuable insights into the intricacies of Cobot manufacturing. The engineer shares some trade secrets and useful techniques that could improve your combat performance. These nuggets of wisdom could be just what you need to gain an edge in the upcoming battles.
-Not only do you walk away with newfound knowledge, but the factory manager is also impressed by your genuine interest in their work. As a token of appreciation for your enthusiasm, they offer you a generous stack of Credits to spend on upgrades or other essential items. Grateful for the unexpected reward, you leave the factory with a spring in your step and a sense of camaraderie with the skilled engineers.</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">
-BITS:
-Did you feel appreciated for the first time in your life? Aww.
-Outcome:
--Gained X HP, Earned X Credits</t>
-    </r>
-  </si>
-  <si>
-    <t>@xxx embarks on a factory tour in Cobot's Steam Arena and gains both valuable insights into Cobot manufacturing and a generous stack of Credits from the impressed factory manager.
-Outcome:
--Gained X HP, Earned X Credits</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>Scenario:
-With a determined look in your eyes, you step onto the sprawling training grounds of Cobot's Steam Arena (sponsored by BITS Artificial Services). The training ground is a hub of activity, with pilots and their Cobots honing their skills, pushing their limits, and preparing for upcoming battles.
-As you join the training session, you find yourself partnered with an experienced pilot known for their exceptional combat prowess. The seasoned pilot is impressed by your dedication and agrees to spar with you, offering valuable guidance throughout the practice session.
-In the intense battle that follows, you give your all, using every trick and technique you've learned over the years. The experienced pilot challenges you to adapt, improvise, and think strategically, pushing you to the limit. Through the spirited contest, you gain valuable combat experience, and your reflexes sharpen considerably.
-Recognizing your progress and determination, the seasoned pilot commends your efforts and shares a few of their most effective strategies. Their guidance proves invaluable, providing you with new approaches to confront your adversaries in the arena.
-As the training session comes to an end, you feel a surge of newfound confidence and pride in your abilities. The experience has not only honed your combat skills but also renewed your spirit for the battles ahead. Grateful for the valuable training and mentorship, you express your thanks to the experienced pilot.</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">
-BITS:
-Well, I am impressed. You look powerful, determined, and intimidating. You may actually prove deadly to your opponents after all. I'm impressed, indeed. 
-Outcome:
--Regerenated two EPs</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx engages in a spirited training session on the training grounds of Cobot's Steam Arena. The mentorship of an experienced pilot not only sharpens his combat skills but also regenerates two EPs.
-Outcome:
--Regerenated two EPs</t>
   </si>
   <si>
     <r>
@@ -1341,7 +1448,7 @@
 BITS:
 Did you see me in the simulation? Yes, I was that perfect bot sitting in the sky box, booing you relentlessly.
 Outcome:
--Gained X HP, Regenerated an EP</t>
+-Gained 40 HP, Regenerated an EP</t>
     </r>
   </si>
   <si>
@@ -1358,12 +1465,11 @@
         <color theme="1"/>
         <sz val="7.0"/>
       </rPr>
-      <t xml:space="preserve">Scenario:
-After a rigorous training session at the Cobot's Steam Arena (sponsored by BITS Artificial Services), your stomach growls with hunger. You head to the bustling food court, a culinary paradise offering a wide array of delicious treats to satiate your appetite.
-As you browse through the various food stalls, the aromas of tantalizing dishes envelop your senses. It's a tough decision to make with so many mouthwatering options, but eventually, you settle on a hearty and nutritious meal that promises to rejuvenate your energy.
-With your plate in hand, you find a cozy corner to enjoy your well-deserved feast. Each bite fills you with satisfaction, and you feel your body being revitalized as the nourishing flavors work their magic. The meal not only pleases your taste buds but also serves as a perfect recovery after your intense training session.
-As you savor the last morsel, you feel a renewed sense of vigor and strength coursing through your circuits. The food court's culinary delights have not only satisfied your hunger but also reinvigorated your body, leaving you ready to face any challenges that lie ahead.
-</t>
+      <t>Scenario:
+As you venture into the vast and bustling factories within Cobot's Steam Arena (sponsored by BITS Artificial Services), you find yourself amidst an impressive display of cutting-edge machinery and skilled technicians working tirelessly to produce the latest innovations in Cobot technology.
+Intrigued by the mesmerizing assembly lines and state-of-the-art production processes, you strike up a conversation with one of the friendly engineers. Impressed by your passion for Cobots and the arena, the engineer decides to show you around and offer some insider tips.
+As you explore the inner workings of the factory, you gain valuable insights into the intricacies of Cobot manufacturing. The engineer shares some trade secrets and useful techniques that could improve your combat performance. These nuggets of wisdom could be just what you need to gain an edge in the upcoming battles.
+Not only do you walk away with newfound knowledge, but the factory manager is also impressed by your genuine interest in their work. As a token of appreciation for your enthusiasm, they offer you a generous stack of Credits to spend on upgrades or other essential items. Grateful for the unexpected reward, you leave the factory with a spring in your step and a sense of camaraderie with the skilled engineers.</t>
     </r>
     <r>
       <rPr>
@@ -1371,17 +1477,17 @@
         <color theme="1"/>
         <sz val="7.0"/>
       </rPr>
-      <t>BITS:
-Oh, Leia's Spoonful Happiness is a great place to eat. Sometimes I wish I could eat food. But again, being perfect is not easy, and being unable to eat food is a small price for being perfect.
+      <t xml:space="preserve">
+BITS:
+Did you feel appreciated for the first time in your life? Aww.
 Outcome:
--Gained X HP</t>
+-Gained 40 HP, Earned 100 Credits</t>
     </r>
   </si>
   <si>
-    <t>Feed:
-@xxx indulges in a delightful meal at the food court, reaping the rewards of a nourishing feast. HP levels surge as the pilot's body rejuvenates.
+    <t>@xxx embarks on a factory tour in Cobot's Steam Arena and gains both valuable insights into Cobot manufacturing and a generous stack of Credits from the impressed factory manager.
 Outcome:
--Gained X HP</t>
+-Gained X HP, Earned X Credits</t>
   </si>
   <si>
     <r>
@@ -1408,7 +1514,7 @@
 BITS:
 Well, even I haven't expected that outcome. Do you want to share your extra Credits with me or?
 Outcome:
--Earned X Credits</t>
+-Earned 300 Credits</t>
     </r>
   </si>
   <si>
@@ -1416,108 +1522,6 @@
 @xxx emerges from the armory, clutching a powerful energy blaster—a testament to their wise decision-making. With new Credits in hand, the pilot stands ready to face any challenge that dares cross their path.
 Outcome:
 -Earned X Credits</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>Scenario:
-As your Cobot docks at the charging station in the heart of the Cobot's Steam Arena (sponsored by BITS Artificial Services), you notice a peculiar sight. A group of friendly engineers, clad in colorful overalls, are showcasing their latest invention—a state-of-the-art energy amplifier.
-Intrigued by their enthusiasm and the potential benefits it could bring to your Cobot's performance, you decide to volunteer as a test pilot for the energy amplifier. With a mix of excitement and anticipation, you watch as the engineers carefully install the device on your Cobot.
-As the energy amplifier hums to life, you feel an immediate surge of power coursing through your circuits. The boost in energy is exhilarating, and you can't help but let out a cheer as you test your Cobot's newfound capabilities. It's as if you've been granted a temporary upgrade, and the thrill of this enhanced performance fills you with confidence.
-In the midst of your test run, a crowd of curious onlookers gathers, including some fellow pilots and even a few high-ranking officials from the arena. Your impressive demonstration draws cheers and applause, and the engineers' faces beam with pride.
-After the successful test, the engineers express their gratitude for your help and offer you the energy amplifier as a gift for your participation. They believe it will serve you well in your future battles and provide an edge in the fiercely competitive arena.</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">
-BITS:
-Do you have a permit for that upgrade? Do you have the necessary papers? DO YOU? 
-Outcome:
--Gained X HP, Earned X Credits, Regenerated an EP</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx electrifies the charging station with a dazzling display of power, courtesy of the engineers' latest energy amplifier. His Cobot surges with energy, and the crowd gathers in awe of the thrilling spectacle. In recognition of his contribution, the engineers bestow the coveted energy amplifier and a handful of credits.
-Outcome:
--Gained X HP, Earned X Credits, Regenerated an EP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">Scenario:
-In the farthest reaches of the Cobot's Steam Arena (sponsored by BITS Artificial Services), hidden behind layers of advanced holographic barriers, lies the enigmatic "Nebula Nexus." This elusive nexus is rumored to be an ancient source of boundless energy, capable of revitalizing even the most drained Cobots.
-As you embark on a daring expedition to locate the Nebula Nexus, whispers of its existence become more fervent. Many pilots have sought its rejuvenating powers, but few have ever returned to tell the tale. Undeterred, you follow a cryptic trail of clues left by those who came before, your determination fueling your journey.
-After navigating through treacherous terrain and solving intricate puzzles, you finally stand before the mesmerizing Nebula Nexus. A pulsating, iridescent cloud of energy envelops you and your Cobot, infusing you both with renewed vitality.
-In the embrace of the Nebula Nexus, time seems to slow, and you can feel every fiber of your Cobot's being reinvigorating. Your EPs, once depleted, now surge back to full capacity, as if the nexus itself grants you the power to push beyond your limits.
-With your Cobot revitalized and your spirits lifted, you step away from the Nebula Nexus, awestruck by the profound experience. You can't help but feel a sense of connection to this ancient source of energy, as if it recognizes and rewards the worthy pilots who seek its blessings.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>BITS:
-Nebula Nexus, have you been there? If so, how are you still alive? Even I don't prefer to explore that mysterious place. Yes, this dimension is my creation, but Nebula Nexus is a total mystery, even to me.
-Outcome: 
--Regerenated all EPs</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx embarks on a perilous quest to discover the legendary Nebula Nexus. A place of mystical energy said to restore the weary. The rewards of courage and determination are truly grand!
-Outcome:
--Regerenated all EPs</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">Scenario:
-As you venture into the heart of the Cobot's Steam Arena (sponsored by BITS Artificial Services), an air of mystery surrounds you. Rumors of a hidden armory have reached your ears—an armory said to house powerful and rare relics, awaiting the touch of a worthy pilot.
-Guided by an old map found in the Mechanic Museum, you traverse through dimly lit corridors until you stumble upon a concealed entrance. The ancient door creaks open, revealing an awe-inspiring chamber filled with artifacts of the past.
-Among the myriad of gleaming weaponry, your eyes fall upon a pedestal adorned with an extraordinary device—the EMP Paralyzer. Its sleek design and pulsating energy beckon to you, resonating with an almost sentient allure.
-Hesitation gives way to determination as you reach out and grasp the EMP Paralyzer. A jolt of energy courses through your veins, and you can feel the newfound power at your fingertips. The device is a marvel of technology, capable of temporarily immobilizing enemy Cobots, giving you a crucial advantage in battle.
-You can't help but marvel at your newfound acquisition, knowing that the EMP Paralyzer will undoubtedly turn the tides of future battles in your favor. With this ancient relic in your possession, you are now ready to face any challenge that dares to cross your path.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>BITS:
-Ah, nothing feels better than a successful treasure hunt, right? I love treasure hunts myself; if you have more hunts planned, I'll gladly tag along with you. 
-Outcome:
--Acquired EMP Paralyzer (weapon)</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx discovers an ancient armory hidden within the labyrinth of the Cobot's Steam Arena. Among the treasures, @xxx unearths the legendary EMP Paralyzer—a powerful weapon capable of stunning enemy Cobots.
-Outcome:
--Acquired EMP Paralyzer (weapon)</t>
   </si>
   <si>
     <r>
@@ -1554,6 +1558,109 @@
 @xxx embarks on a thrilling quest to uncover the legendary Quantum Armor hidden within the depths of the Cobot's Steam Arena. Through perseverance and valor, the pilot crafts the celestial armor.
 Outcome:
 -Acquired Quantum Armor (armor)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>Scenario:
+As your Cobot docks at the charging station in the heart of the Cobot's Steam Arena (sponsored by BITS Artificial Services), you notice a peculiar sight. A group of friendly engineers, clad in colorful overalls, are showcasing their latest invention—a state-of-the-art energy amplifier.
+Intrigued by their enthusiasm and the potential benefits it could bring to your Cobot's performance, you decide to volunteer as a test pilot for the energy amplifier. With a mix of excitement and anticipation, you watch as the engineers carefully install the device on your Cobot.
+As the energy amplifier hums to life, you feel an immediate surge of power coursing through your circuits. The boost in energy is exhilarating, and you can't help but let out a cheer as you test your Cobot's newfound capabilities. It's as if you've been granted a temporary upgrade, and the thrill of this enhanced performance fills you with confidence.
+In the midst of your test run, a crowd of curious onlookers gathers, including some fellow pilots and even a few high-ranking officials from the arena. Your impressive demonstration draws cheers and applause, and the engineers' faces beam with pride.
+After the successful test, the engineers express their gratitude for your help and offer you the energy amplifier as a gift for your participation. They believe it will serve you well in your future battles and provide an edge in the fiercely competitive arena.</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">
+BITS:
+Do you have a permit for that upgrade? Do you have the necessary papers? DO YOU? 
+Outcome:
+-Gained 33 HP, Earned 150 Credits, Regenerated an EP</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx electrifies the charging station with a dazzling display of power, courtesy of the engineers' latest energy amplifier. His Cobot surges with energy, and the crowd gathers in awe of the thrilling spectacle. In recognition of his contribution, the engineers bestow the coveted energy amplifier and a handful of credits.
+Outcome:
+-Gained X HP, Earned X Credits, Regenerated an EP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">Scenario:
+As you venture into the heart of the Cobot's Steam Arena (sponsored by BITS Artificial Services), an air of mystery surrounds you. Rumors of a hidden armory have reached your ears—an armory said to house powerful and rare relics, awaiting the touch of a worthy pilot.
+Guided by an old map found in the Mechanic Museum, you traverse through dimly lit corridors until you stumble upon a concealed entrance. The ancient door creaks open, revealing an awe-inspiring chamber filled with artifacts of the past.
+Among the myriad of gleaming weaponry, your eyes fall upon a pedestal adorned with an extraordinary device—the EMP Paralyzer. Its sleek design and pulsating energy beckon to you, resonating with an almost sentient allure.
+Hesitation gives way to determination as you reach out and grasp the EMP Paralyzer. A jolt of energy courses through your veins, and you can feel the newfound power at your fingertips. The device is a marvel of technology, capable of temporarily immobilizing enemy Cobots, giving you a crucial advantage in battle.
+You can't help but marvel at your newfound acquisition, knowing that the EMP Paralyzer will undoubtedly turn the tides of future battles in your favor. With this ancient relic in your possession, you are now ready to face any challenge that dares to cross your path.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>BITS:
+Ah, nothing feels better than a successful treasure hunt, right? I love treasure hunts myself; if you have more hunts planned, I'll gladly tag along with you. 
+Outcome:
+-Acquired EMP Paralyzer (weapon)</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx discovers an ancient armory hidden within the labyrinth of the Cobot's Steam Arena. Among the treasures, @xxx unearths the legendary EMP Paralyzer—a powerful weapon capable of stunning enemy Cobots.
+Outcome:
+-Acquired EMP Paralyzer (weapon)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t>Scenario:
+Within the vast expanse of Cobot's Steam Arena (sponsored by BITS Artificial Services), you stumble upon a hidden corner known as "Astral Antiquities." The shop's entrance is adorned with twinkling constellations, and a mysterious figure beckons you with a cosmic aura.
+As you venture into the otherworldly emporium, you encounter Orion, the enigmatic celestial collector. His eyes glimmer like distant stars, and his voice resonates with the echoes of galaxies.
+Orion leads you through an array of interstellar artifacts, each with its own fabled history. But among them, your attention is drawn to the "Astro-Matter Manipulator." This extraordinary device is said to harness the power of cosmic forces, capable of transforming your armor into the extraordinary "Gravitational Absorber."
+With a mischievous glint in his eyes, Orion offers you a chance to wield the awe-inspiring abilities of the "Gravitational Absorber." It promises to alter the fabric of space around you, rendering you nigh invulnerable to your opponents' assaults.
+Unable to resist the allure of celestial might, you accept Orion's offer and integrate the "Astro-Matter Manipulator" into your Cobot's armor. The sensation is surreal as you feel the very laws of gravity shifting around you.
+The "Gravitational Absorber" now encases your Cobot, a testament to the harmonious blend of technology and cosmic energies. As you step back into the arena, your foes are astounded by the newfound resilience emanating from your armored form.</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="7.0"/>
+      </rPr>
+      <t xml:space="preserve">
+BITS:
+Orion is the best medium that you can encounter by far! Not only in this dimension but in every single dimension! Did you know that I am supposed to be a human like you, but because I am perfect in every possible way, it was impossible for me to be just a human? It is a fact based on my horoscope.
+Outcome:
+Upgraded your armor to Gravitational Absorber</t>
+    </r>
+  </si>
+  <si>
+    <t>Feed:
+@xxx embarks on a cosmic journey to "Astral Antiquities," where he encounters Orion, the celestial collector. In awe, @xxx integrates the "Astro-Matter Manipulator" into their armor, and behold, the birth of the extraordinary "Gravitational Absorber."
+Outcome:
+-Upgraded your armor to Gravitational Absorber</t>
   </si>
   <si>
     <r>
@@ -1607,112 +1714,6 @@
 @xxx stumbles upon the elusive black market shop within the depths of the Cobot's Steam Arena, where the legendary Super Duper Planet Blower awaits its destined owner.
 Outcome:
 -Upgraded your weapon to Super Duper Planet Blower (weapon)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>Scenario:
-Within the vast expanse of Cobot's Steam Arena (sponsored by BITS Artificial Services), you stumble upon a hidden corner known as "Astral Antiquities." The shop's entrance is adorned with twinkling constellations, and a mysterious figure beckons you with a cosmic aura.
-As you venture into the otherworldly emporium, you encounter Orion, the enigmatic celestial collector. His eyes glimmer like distant stars, and his voice resonates with the echoes of galaxies.
-Orion leads you through an array of interstellar artifacts, each with its own fabled history. But among them, your attention is drawn to the "Astro-Matter Manipulator." This extraordinary device is said to harness the power of cosmic forces, capable of transforming your armor into the extraordinary "Gravitational Absorber."
-With a mischievous glint in his eyes, Orion offers you a chance to wield the awe-inspiring abilities of the "Gravitational Absorber." It promises to alter the fabric of space around you, rendering you nigh invulnerable to your opponents' assaults.
-Unable to resist the allure of celestial might, you accept Orion's offer and integrate the "Astro-Matter Manipulator" into your Cobot's armor. The sensation is surreal as you feel the very laws of gravity shifting around you.
-The "Gravitational Absorber" now encases your Cobot, a testament to the harmonious blend of technology and cosmic energies. As you step back into the arena, your foes are astounded by the newfound resilience emanating from your armored form.</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">
-BITS:
-Orion is the best medium that you can encounter by far! Not only in this dimension but in every single dimension! Did you know that I am supposed to be a human like you, but because I am perfect in every possible way, it was impossible for me to be just a human? It is a fact based on my horoscope.
-Outcome:
-Upgraded your armor to Gravitational Absorber</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx embarks on a cosmic journey to "Astral Antiquities," where he encounters Orion, the celestial collector. In awe, @xxx integrates the "Astro-Matter Manipulator" into their armor, and behold, the birth of the extraordinary "Gravitational Absorber."
-Outcome:
--Upgraded your armor to Gravitational Absorber</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>Scenario:
-Amidst the hustle and bustle of the Hospital Wing in Cobot's Steam Arena (sponsored by BITS Artificial Services), you come across an intriguing medical research display. A renowned scientist, Dr. Aurora, stands by the exhibit, her eyes gleaming with curiosity and passion.
-Dr. Aurora invites you to explore her groundbreaking research on advanced bio-neural technology. As you delve deeper into the intricacies of her work, you uncover an innovative device known as the "Neural Resonance Enhancer."
-This extraordinary invention has the ability to enhance your neural connections, granting you greater mental acuity and reflexes. Dr. Aurora eagerly offers you the chance to experience the "Neural Resonance Enhancer" firsthand.
-With a sense of excitement, you agree to participate in her experiment. Dr. Aurora carefully connects the device to your Cobot's neural interface, and you feel a subtle surge of energy coursing through your circuits.
-The "Neural Resonance Enhancer" initiates a synchronized resonance with your consciousness, awakening dormant potential within. You sense a newfound clarity and focus, as if the entire arena's secrets lay bare before you.
-As you leave Dr. Aurora's display, you find your thoughts sharper and your responses quicker. The "Neural Resonance Enhancer" has left a lasting impact on your Cobot's neural pathways, granting you an advantage in Spintop's Cobot Rumble.</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">
-BITS:
-I did not know that you were so eager to join the experiments as a subject without knowing the outcome. I am creating a new dimension where organic life is impossible to sustain. Would you like to give it a spin?
-Outcome:
--Regenerated an EP</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx ventures into the Hospital Wing, where he encounters Dr. Aurora and her revolutionary "Neural Resonance Enhancer." Eager to explore its potential, @xxx undergoes the experiment and emerges with heightened mental acuity.
-Outcome:
--Regenerated an EP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>Scenario:
-Amidst the aroma of delectable delicacies and the chatter of fellow pilots in Cobot's Steam Arena (sponsored by BITS Artificial Services), you find yourself at the bustling Food Court, contemplating your dining options.
-As you peruse the various food stalls, your attention is drawn to an unassuming vending machine tucked in the corner. Unlike the others, this vending machine seems to radiate an aura of intelligence, with blinking lights and holographic equations swirling around it.
-Intrigued, you approach the machine, and it greets you with a cheerful holographic display. "Welcome, esteemed pilot! I am the Gourmettron 9000, an AI-powered vending machine with a passion for gastronomy and brain teasers."
-The Gourmettron 9000 offers you a unique proposition - a culinary challenge! It boasts a collection of exotic dishes from across the universe, each connected to a riddle or puzzle. If you successfully solve the riddle, the Gourmettron 9000 will treat you to an extraordinary meal and reward you with a generous amount of Credits.
-Eager for the opportunity, you accept the challenge and prepare to put your wits to the test. The Gourmettron 9000 presents you with an intricate puzzle, and you delve into the enigma, savoring the mental stimulation.
-With each step towards the solution, you can almost taste the victory. Moments later, your problem-solving prowess triumphs, and the Gourmettron 9000 commends you with a holographic applause.
-True to its word, the vending machine dispenses a delectable feast, and you indulge in the gastronomic delight. As you savor the culinary masterpiece, the Gourmettron 9000 credits your account with a generous sum, acknowledging your brilliance and culinary appreciation.</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t xml:space="preserve">
-BITS:
-There are 47,989 different robots, bots, and drones in this artificial dimension that I've created. I programmed nearly half of them specifically to be puzzling and teasing. Out of 23,259 mechanic automaton riddle givers, you've found the most merciful one. Congratulations.
-Outcome:
--Earned X Credits</t>
-    </r>
-  </si>
-  <si>
-    <t>Feed:
-@xxx faces an intellectual challenge at the Food Court as he encounters the Gourmettron 9000, an AI-powered vending machine. By skillfully solving the riddle, @xxx earns a generous reward of Credits and indulges in an exquisite feast.
-Outcome:
--Earned X Credits</t>
   </si>
   <si>
     <r>
@@ -2453,6 +2454,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="9.0"/>
       <color theme="1"/>
@@ -2470,18 +2483,6 @@
       <sz val="7.0"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -2784,22 +2785,22 @@
     <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -8507,58 +8508,68 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="15"/>
+      <c r="A2" s="15">
+        <v>32.0</v>
+      </c>
       <c r="B2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19">
-        <v>24.0</v>
-      </c>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="15">
+        <v>33.0</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20" t="s">
+      <c r="A4" s="15">
+        <v>34.0</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="18">
+        <v>36.0</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="15"/>
+      <c r="A6" s="15">
+        <v>35.0</v>
+      </c>
       <c r="B6" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="16" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="18">
+        <v>37.0</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C7" s="20" t="s">
@@ -8566,8 +8577,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="15">
+        <v>38.0</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -8575,27 +8588,33 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="15">
+        <v>39.0</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="15">
+        <v>40.0</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="16" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="18">
+        <v>41.0</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -8603,78 +8622,90 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="15">
+        <v>42.0</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="15">
+        <v>43.0</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="15">
+        <v>44.0</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="16" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="15">
+        <v>45.0</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="16" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="15">
-        <v>50.0</v>
+        <v>46.0</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="16" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="19">
+      <c r="A17" s="15">
+        <v>47.0</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="15">
+        <v>48.0</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="18">
         <v>49.0</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="16" t="s">
         <v>102</v>
       </c>
     </row>
@@ -13584,6 +13615,11 @@
       <c r="C1000" s="22"/>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$C$1000">
+    <sortState ref="A1:C1000">
+      <sortCondition ref="A1:A1000"/>
+    </sortState>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: add random encounter text emojis
</commit_message>
<xml_diff>
--- a/data/randoms.xlsx
+++ b/data/randoms.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="283">
   <si>
     <r>
       <rPr>
@@ -133,12 +133,6 @@
   <si>
     <t>Alt banner:
 Register for Spintop's Cobot Rumble on Discord, be the ultimate pilot and win $1500!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inactivity: </t>
-  </si>
-  <si>
-    <t>Genel bildirim metinleri:</t>
   </si>
   <si>
     <t>The Story of the Encounter (DM)</t>
@@ -1758,12 +1752,16 @@
       </rPr>
       <t xml:space="preserve">
 BITS:
-You look good in that pink and shiny knight armor. However, my favorite version of you is the one who keeps dancing nonstop in an intergalactic talent show. Now, you are officially humiliated in front of billions of aliens.</t>
+You look good in that pink and shiny knight armor. However, my favorite version of you is the one who keeps dancing nonstop in an intergalactic talent show. Now, you are officially humiliated in front of billions of aliens.
+Outcome:
+Nothing has happened that affected the outcome.</t>
     </r>
   </si>
   <si>
     <t>Feed:
-@xxx stumbles upon the enigmatic Multiverse Mirror Gallery, a room filled with mirrors reflecting infinite versions of himself in diverse realities. The journey through parallel dimensions becomes a moment of profound introspection, unveiling the marvels of existence and the uniqueness of our intrepid pilot.</t>
+@xxx stumbles upon the enigmatic Multiverse Mirror Gallery, a room filled with mirrors reflecting infinite versions of himself in diverse realities. The journey through parallel dimensions becomes a moment of profound introspection, unveiling the marvels of existence and the uniqueness of our intrepid pilot.
+Outcome:
+Nothing has happened that affected the outcome.</t>
   </si>
   <si>
     <r>
@@ -1789,12 +1787,16 @@
       </rPr>
       <t xml:space="preserve">
 BITS:
-If I remember correctly, Professor Wunderbar is looking for clowns to hire. Let me know if you're interested. I will gladly speak with Professor on behalf of you.</t>
+If I remember correctly, Professor Wunderbar is looking for clowns to hire. Let me know if you're interested. I will gladly speak with Professor on behalf of you.
+Outcome:
+Nothing has happened that affected the outcome.</t>
     </r>
   </si>
   <si>
     <t>Feed:
-@xxx steps into Professor Wunderbar's Circus of Wonders, encountering a mind-boggling array of acts and a Quantum Fortune Machine that reveals improbable visions of cobot feats. The circus leaves everyone in awe, cherishing the magic-filled trinkets that serve as keepsakes of the fantastical experience.</t>
+@xxx steps into Professor Wunderbar's Circus of Wonders, encountering a mind-boggling array of acts and a Quantum Fortune Machine that reveals improbable visions of cobot feats. The circus leaves everyone in awe, cherishing the magic-filled trinkets that serve as keepsakes of the fantastical experience.
+Outcome:
+Nothing has happened that affected the outcome.</t>
   </si>
   <si>
     <r>
@@ -1821,12 +1823,16 @@
       </rPr>
       <t xml:space="preserve">
 BITS:
-Do not panic, but I've closed the portal behind your back. No need to get mad; you looked delighted, and you know me, all I want is your happiness.</t>
+Do not panic, but I've closed the portal behind your back. No need to get mad; you looked delighted, and you know me, all I want is your happiness.
+Outcome:
+Nothing has happened that affected the outcome.</t>
     </r>
   </si>
   <si>
     <t>Feed:
-@xxx embarks on a surreal adventure through a holographic portal, discovering a mesmerizing alternate dimension. Encounters cobots with majestic wings, playful crystal creatures, and a fountain of radiant rejuvenation that revitalizes the spirit.</t>
+@xxx embarks on a surreal adventure through a holographic portal, discovering a mesmerizing alternate dimension. Encounters cobots with majestic wings, playful crystal creatures, and a fountain of radiant rejuvenation that revitalizes the spirit.
+Outcome:
+Nothing has happened that affected the outcome.</t>
   </si>
   <si>
     <r>
@@ -1851,12 +1857,16 @@
       </rPr>
       <t xml:space="preserve">
 BITS:
-Hah, we found your true profession at last. I knew Cobot battling wasn't for you.</t>
+Hah, we found your true profession at last. I knew Cobot battling wasn't for you.
+Outcome:
+Nothing has happened that affected the outcome.</t>
     </r>
   </si>
   <si>
     <t>Feed:
-@xxx takes a whimsical detour into the world of the "Jingle Jesters," a troupe of playful cobots who put on a hilarious and heartwarming performance. Laughter fills the air as the pilot joins in the merriment, dancing with the jesters and embracing the spirit of camaraderie.</t>
+@xxx takes a whimsical detour into the world of the "Jingle Jesters," a troupe of playful cobots who put on a hilarious and heartwarming performance. Laughter fills the air as the pilot joins in the merriment, dancing with the jesters and embracing the spirit of camaraderie.
+Outcome:
+Nothing has happened that affected the outcome.</t>
   </si>
   <si>
     <t>Scenario:
@@ -1866,11 +1876,15 @@
 The carvings seem to come alive, narrating snippets of history, prophetic visions, and riddles that challenge the mind. Each step brings new revelations and insights, as if the corridor itself is a sentient being, eager to share its secrets with the curious wanderer.
 The enigmatic symbols and messages leave you with a sense of wonder and awe, and you find yourself drawn deeper into the heart of the Whispering Corridor, hungry for more knowledge and understanding.
 BITS:
-Be careful now; it would be a pity if you lost your way and got stuck in that alley for eternity. I would certainly be devastated. Yes.</t>
+Be careful now; it would be a pity if you lost your way and got stuck in that alley for eternity. I would certainly be devastated. Yes.
+Outcome:
+Nothing has happened that affected the outcome.</t>
   </si>
   <si>
     <t>Feed:
-@xxx delves into the mystical "Whispering Corridor," a secluded passage in the heart of Cobot's Steam Arena, said to reveal secrets and hidden truths to those who dare to enter. Mesmerized by the enigmatic carvings and cryptic messages, the pilot embarks on a journey of discovery, delving deeper into the mysteries of the ancient corridor.</t>
+@xxx delves into the mystical "Whispering Corridor," a secluded passage in the heart of Cobot's Steam Arena, said to reveal secrets and hidden truths to those who dare to enter. Mesmerized by the enigmatic carvings and cryptic messages, the pilot embarks on a journey of discovery, delving deeper into the mysteries of the ancient corridor.
+Outcome:
+Nothing has happened that affected the outcome.</t>
   </si>
   <si>
     <t>Scenario:
@@ -2768,9 +2782,6 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -2785,6 +2796,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -3284,16 +3298,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3320,315 +3324,315 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="4">
+      <c r="A4" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="5">
+      <c r="A5" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="6">
+      <c r="A6" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="7">
+      <c r="A7" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="8">
+      <c r="A8" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="7" t="s">
+    <row r="9">
+      <c r="A9" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="7" t="s">
+    <row r="10">
+      <c r="A10" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="6">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    <row r="11">
+      <c r="A11" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="6">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="7" t="s">
+    <row r="12">
+      <c r="A12" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="6">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    <row r="13">
+      <c r="A13" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="6">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="14">
+      <c r="A14" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="6">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="15">
+      <c r="A15" s="5">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="6">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="7" t="s">
+    <row r="16">
+      <c r="A16" s="5">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="6">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="7" t="s">
+    <row r="17">
+      <c r="A17" s="5">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="B17" s="7" t="s">
+    <row r="18">
+      <c r="A18" s="5">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="6">
-        <v>17.0</v>
-      </c>
-      <c r="B18" s="7" t="s">
+    <row r="19">
+      <c r="A19" s="5">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="6">
-        <v>18.0</v>
-      </c>
-      <c r="B19" s="7" t="s">
+    <row r="20">
+      <c r="A20" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="6">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="7" t="s">
+    <row r="21">
+      <c r="A21" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6">
-        <v>20.0</v>
-      </c>
-      <c r="B21" s="7" t="s">
+      <c r="J21" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="7" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="C22" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="6">
-        <v>21.0</v>
-      </c>
-      <c r="B22" s="7" t="s">
+    <row r="23">
+      <c r="A23" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="6">
-        <v>22.0</v>
-      </c>
-      <c r="B23" s="7" t="s">
+    <row r="24">
+      <c r="A24" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="6">
-        <v>23.0</v>
-      </c>
-      <c r="B24" s="7" t="s">
+    <row r="25">
+      <c r="A25" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="6">
-        <v>24.0</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="26">
+      <c r="A26" s="5">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="6">
-        <v>25.0</v>
-      </c>
-      <c r="B26" s="7" t="s">
+    <row r="27">
+      <c r="A27" s="5">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="6">
-        <v>26.0</v>
-      </c>
-      <c r="B27" s="7" t="s">
+    <row r="28">
+      <c r="A28" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="6">
-        <v>27.0</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="29">
@@ -8525,10 +8529,10 @@
     <row r="1">
       <c r="A1" s="12"/>
       <c r="B1" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -8536,13 +8540,13 @@
         <v>32.0</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3">
@@ -8550,10 +8554,10 @@
         <v>33.0</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -8561,10 +8565,10 @@
         <v>34.0</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -8572,10 +8576,10 @@
         <v>36.0</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -8583,10 +8587,10 @@
         <v>35.0</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
@@ -8594,10 +8598,10 @@
         <v>37.0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
@@ -8605,10 +8609,10 @@
         <v>38.0</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
@@ -8616,22 +8620,22 @@
         <v>39.0</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="8"/>
+        <v>80</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="15">
         <v>40.0</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
@@ -8639,10 +8643,10 @@
         <v>41.0</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
@@ -8650,10 +8654,10 @@
         <v>42.0</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13">
@@ -8661,10 +8665,10 @@
         <v>43.0</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14">
@@ -8672,10 +8676,10 @@
         <v>44.0</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
@@ -8683,10 +8687,10 @@
         <v>45.0</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
@@ -8694,10 +8698,10 @@
         <v>46.0</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
@@ -8705,10 +8709,10 @@
         <v>47.0</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -8716,10 +8720,10 @@
         <v>48.0</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -8727,16 +8731,16 @@
         <v>49.0</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="21"/>
       <c r="B20" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="23"/>
     </row>
@@ -13669,50 +13673,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7">
@@ -13771,50 +13775,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -13838,28 +13842,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>126</v>
       </c>
       <c r="D1" s="30"/>
       <c r="E1" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="31">
         <v>1.0</v>
@@ -13869,7 +13873,7 @@
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F2" s="31">
         <v>0.1</v>
@@ -13880,7 +13884,7 @@
     </row>
     <row r="3">
       <c r="A3" s="31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B3" s="31">
         <v>2.0</v>
@@ -13890,7 +13894,7 @@
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F3" s="31">
         <v>0.2</v>
@@ -13901,7 +13905,7 @@
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4" s="31">
         <v>3.0</v>
@@ -13911,7 +13915,7 @@
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F4" s="31">
         <v>0.3</v>
@@ -13922,7 +13926,7 @@
     </row>
     <row r="5">
       <c r="A5" s="31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" s="31">
         <v>4.0</v>
@@ -13932,7 +13936,7 @@
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F5" s="31">
         <v>0.4</v>
@@ -13943,7 +13947,7 @@
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6" s="31">
         <v>5.0</v>
@@ -13953,7 +13957,7 @@
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F6" s="31">
         <v>0.5</v>
@@ -13964,7 +13968,7 @@
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B7" s="31">
         <v>6.0</v>
@@ -13979,7 +13983,7 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B8" s="31">
         <v>7.0</v>
@@ -13994,7 +13998,7 @@
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B9" s="31">
         <v>8.0</v>
@@ -14009,7 +14013,7 @@
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B10" s="31">
         <v>9.0</v>
@@ -14024,7 +14028,7 @@
     </row>
     <row r="11">
       <c r="A11" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B11" s="31">
         <v>10.0</v>
@@ -14060,7 +14064,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
@@ -14070,10 +14074,10 @@
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" s="34"/>
       <c r="G3" s="37"/>
@@ -14081,10 +14085,10 @@
     </row>
     <row r="4">
       <c r="A4" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D4" s="37"/>
       <c r="G4" s="37"/>
@@ -14092,10 +14096,10 @@
     </row>
     <row r="5">
       <c r="A5" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D5" s="37"/>
       <c r="G5" s="37"/>
@@ -14103,10 +14107,10 @@
     </row>
     <row r="6">
       <c r="A6" s="35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D6" s="37"/>
       <c r="G6" s="37"/>
@@ -14114,10 +14118,10 @@
     </row>
     <row r="7">
       <c r="A7" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D7" s="37"/>
       <c r="G7" s="37"/>
@@ -14125,10 +14129,10 @@
     </row>
     <row r="8">
       <c r="A8" s="42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D8" s="37"/>
     </row>
@@ -14137,7 +14141,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11">
@@ -14145,50 +14149,50 @@
     </row>
     <row r="12">
       <c r="A12" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -14222,42 +14226,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C1" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="F1" s="51" t="s">
         <v>152</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="D2" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="E2" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="F2" s="55" t="s">
         <v>168</v>
-      </c>
-      <c r="E2" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="55" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3">
@@ -14282,22 +14286,22 @@
     </row>
     <row r="5">
       <c r="A5" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="D5" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="E5" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="F5" s="55" t="s">
         <v>174</v>
-      </c>
-      <c r="E5" s="54" t="s">
-        <v>175</v>
-      </c>
-      <c r="F5" s="55" t="s">
-        <v>176</v>
       </c>
       <c r="H5" s="37"/>
       <c r="J5" s="37"/>
@@ -14324,22 +14328,22 @@
     </row>
     <row r="8">
       <c r="A8" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="D8" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="E8" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="F8" s="55" t="s">
         <v>180</v>
-      </c>
-      <c r="E8" s="54" t="s">
-        <v>181</v>
-      </c>
-      <c r="F8" s="55" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="9">
@@ -14360,22 +14364,22 @@
     </row>
     <row r="11">
       <c r="A11" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="D11" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="E11" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="F11" s="55" t="s">
         <v>186</v>
-      </c>
-      <c r="E11" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="12">
@@ -14396,22 +14400,22 @@
     </row>
     <row r="14">
       <c r="A14" s="61" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="54" t="s">
         <v>189</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="D14" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="E14" s="54" t="s">
         <v>191</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="F14" s="55" t="s">
         <v>192</v>
-      </c>
-      <c r="E14" s="54" t="s">
-        <v>193</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="15">
@@ -14433,22 +14437,22 @@
     </row>
     <row r="17">
       <c r="A17" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="D17" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="E17" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="F17" s="55" t="s">
         <v>198</v>
-      </c>
-      <c r="E17" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" s="55" t="s">
-        <v>200</v>
       </c>
       <c r="I17" s="64"/>
     </row>
@@ -14472,22 +14476,22 @@
     </row>
     <row r="20">
       <c r="A20" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="D20" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="E20" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="F20" s="55" t="s">
         <v>204</v>
-      </c>
-      <c r="E20" s="54" t="s">
-        <v>205</v>
-      </c>
-      <c r="F20" s="55" t="s">
-        <v>206</v>
       </c>
       <c r="I20" s="65"/>
     </row>
@@ -14509,22 +14513,22 @@
     </row>
     <row r="23">
       <c r="A23" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="53" t="s">
+      <c r="D23" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="E23" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="F23" s="55" t="s">
         <v>210</v>
-      </c>
-      <c r="E23" s="54" t="s">
-        <v>211</v>
-      </c>
-      <c r="F23" s="55" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="24">
@@ -14545,22 +14549,22 @@
     </row>
     <row r="26">
       <c r="A26" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="D26" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="E26" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="F26" s="55" t="s">
         <v>216</v>
-      </c>
-      <c r="E26" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="27">
@@ -14581,22 +14585,22 @@
     </row>
     <row r="29">
       <c r="A29" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="C29" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="B29" s="53" t="s">
+      <c r="D29" s="54" t="s">
         <v>220</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="E29" s="54" t="s">
         <v>221</v>
       </c>
-      <c r="D29" s="54" t="s">
+      <c r="F29" s="55" t="s">
         <v>222</v>
-      </c>
-      <c r="E29" s="54" t="s">
-        <v>223</v>
-      </c>
-      <c r="F29" s="55" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -14630,62 +14634,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="70" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C1" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="E1" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="F1" s="75" t="s">
         <v>152</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="69" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="D2" s="76" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="E2" s="76" t="s">
         <v>227</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="F2" s="77" t="s">
         <v>228</v>
-      </c>
-      <c r="E2" s="76" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="77" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="69" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="D3" s="77" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="E3" s="77" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="F3" s="77" t="s">
         <v>234</v>
-      </c>
-      <c r="E3" s="77" t="s">
-        <v>235</v>
-      </c>
-      <c r="F3" s="77" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="4">
@@ -14698,44 +14702,44 @@
     </row>
     <row r="6">
       <c r="A6" s="67" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="78" t="s">
         <v>237</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="D6" s="78" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="E6" s="78" t="s">
         <v>239</v>
       </c>
-      <c r="D6" s="78" t="s">
+      <c r="F6" s="78" t="s">
         <v>240</v>
-      </c>
-      <c r="E6" s="78" t="s">
-        <v>241</v>
-      </c>
-      <c r="F6" s="78" t="s">
-        <v>242</v>
       </c>
       <c r="H6" s="37"/>
       <c r="J6" s="37"/>
     </row>
     <row r="7">
       <c r="A7" s="67" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="78" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" s="78" t="s">
         <v>243</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="D7" s="78" t="s">
         <v>244</v>
       </c>
-      <c r="C7" s="78" t="s">
+      <c r="E7" s="78" t="s">
         <v>245</v>
       </c>
-      <c r="D7" s="78" t="s">
+      <c r="F7" s="78" t="s">
         <v>246</v>
-      </c>
-      <c r="E7" s="78" t="s">
-        <v>247</v>
-      </c>
-      <c r="F7" s="78" t="s">
-        <v>248</v>
       </c>
       <c r="H7" s="37"/>
       <c r="J7" s="37"/>
@@ -14750,122 +14754,122 @@
     </row>
     <row r="10">
       <c r="A10" s="79" t="s">
+        <v>247</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="78" t="s">
         <v>249</v>
       </c>
-      <c r="B10" s="78" t="s">
+      <c r="D10" s="55" t="s">
         <v>250</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="E10" s="55" t="s">
         <v>251</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="F10" s="55" t="s">
         <v>252</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>253</v>
-      </c>
-      <c r="F10" s="55" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="79" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="78" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="78" t="s">
         <v>255</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="D11" s="78" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="E11" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="F11" s="78" t="s">
         <v>258</v>
-      </c>
-      <c r="E11" s="78" t="s">
-        <v>259</v>
-      </c>
-      <c r="F11" s="78" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="80" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>260</v>
+      </c>
+      <c r="C14" s="78" t="s">
         <v>261</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="D14" s="55" t="s">
         <v>262</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="E14" s="78" t="s">
         <v>263</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="F14" s="55" t="s">
         <v>264</v>
-      </c>
-      <c r="E14" s="78" t="s">
-        <v>265</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="80" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" s="78" t="s">
         <v>267</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="D15" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="E15" s="78" t="s">
         <v>269</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="F15" s="78" t="s">
         <v>270</v>
-      </c>
-      <c r="E15" s="78" t="s">
-        <v>271</v>
-      </c>
-      <c r="F15" s="78" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="81" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="C18" s="78" t="s">
         <v>273</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="D18" s="55" t="s">
         <v>274</v>
       </c>
-      <c r="C18" s="78" t="s">
+      <c r="E18" s="55" t="s">
         <v>275</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="F18" s="55" t="s">
         <v>276</v>
-      </c>
-      <c r="E18" s="55" t="s">
-        <v>277</v>
-      </c>
-      <c r="F18" s="55" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="81" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="D19" s="78" t="s">
         <v>280</v>
       </c>
-      <c r="C19" s="78" t="s">
+      <c r="E19" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="D19" s="78" t="s">
+      <c r="F19" s="78" t="s">
         <v>282</v>
-      </c>
-      <c r="E19" s="78" t="s">
-        <v>283</v>
-      </c>
-      <c r="F19" s="78" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="21">

</xml_diff>